<commit_message>
make new position counter
</commit_message>
<xml_diff>
--- a/students.xlsx
+++ b/students.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isaaccandari/CS/Work/waitlist-app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB8131E1-9C45-0641-AC66-3E9A678644ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34FA6F20-0D62-DB40-955A-B26E01EE8832}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7000" yWindow="4980" windowWidth="28040" windowHeight="17440" xr2:uid="{3CB57614-CEEE-7B4A-9D12-C81DD3693F0A}"/>
+    <workbookView xWindow="-28040" yWindow="2200" windowWidth="28040" windowHeight="17440" xr2:uid="{3CB57614-CEEE-7B4A-9D12-C81DD3693F0A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Name</t>
   </si>
@@ -57,6 +57,12 @@
   </si>
   <si>
     <t>yes</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>Getting Married</t>
   </si>
 </sst>
 </file>
@@ -428,15 +434,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62856E69-D4D8-394A-94BA-9D10EEA124FC}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -446,8 +452,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -457,8 +466,11 @@
       <c r="C2">
         <v>1</v>
       </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -468,8 +480,11 @@
       <c r="C3">
         <v>0</v>
       </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -479,8 +494,11 @@
       <c r="C4">
         <v>1</v>
       </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -489,6 +507,23 @@
       </c>
       <c r="C5">
         <v>1</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Front end version 1
</commit_message>
<xml_diff>
--- a/students.xlsx
+++ b/students.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isaaccandari/CS/Work/waitlist-app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CC2F64C-F402-6448-9CD2-F5C0452F4390}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4856C4B-AFE4-C547-AE50-14A1633B1E60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28040" yWindow="2200" windowWidth="28040" windowHeight="17440" xr2:uid="{3CB57614-CEEE-7B4A-9D12-C81DD3693F0A}"/>
   </bookViews>
@@ -461,7 +461,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -492,7 +492,7 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>2073777</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -509,7 +509,7 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>2071398</v>
       </c>
       <c r="C3">
         <v>0</v>

</xml_diff>

<commit_message>
chang waitlist logic for active users
</commit_message>
<xml_diff>
--- a/students.xlsx
+++ b/students.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isaaccandari/CS/Work/waitlist-app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4856C4B-AFE4-C547-AE50-14A1633B1E60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9D5AEB3-32AA-4449-BC05-57CFDF0E3A67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28040" yWindow="2200" windowWidth="28040" windowHeight="17440" xr2:uid="{3CB57614-CEEE-7B4A-9D12-C81DD3693F0A}"/>
+    <workbookView xWindow="4980" yWindow="2700" windowWidth="34560" windowHeight="15560" xr2:uid="{3CB57614-CEEE-7B4A-9D12-C81DD3693F0A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Name</t>
   </si>
@@ -53,15 +53,6 @@
     <t>Bea</t>
   </si>
   <si>
-    <t>Rice</t>
-  </si>
-  <si>
-    <t>yes</t>
-  </si>
-  <si>
-    <t>no</t>
-  </si>
-  <si>
     <t>Getting Married</t>
   </si>
   <si>
@@ -74,13 +65,34 @@
     <t>08/18/2021</t>
   </si>
   <si>
-    <t>07/18/2022</t>
-  </si>
-  <si>
-    <t>08/18/2022</t>
-  </si>
-  <si>
-    <t>07/18/2023</t>
+    <t>Jeff</t>
+  </si>
+  <si>
+    <t>Lisa</t>
+  </si>
+  <si>
+    <t>Alice</t>
+  </si>
+  <si>
+    <t>Reed</t>
+  </si>
+  <si>
+    <t>Miller</t>
+  </si>
+  <si>
+    <t>09/18/2021</t>
+  </si>
+  <si>
+    <t>10/18/2021</t>
+  </si>
+  <si>
+    <t>11/18/2021</t>
+  </si>
+  <si>
+    <t>12/18/2021</t>
+  </si>
+  <si>
+    <t>01/18/2022</t>
   </si>
 </sst>
 </file>
@@ -458,10 +470,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62856E69-D4D8-394A-94BA-9D10EEA124FC}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -481,10 +493,10 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -492,7 +504,7 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>2073777</v>
+        <v>1</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -501,7 +513,7 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -509,7 +521,7 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>2071398</v>
+        <v>2</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -518,12 +530,12 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -535,12 +547,12 @@
         <v>0</v>
       </c>
       <c r="E4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -552,12 +564,12 @@
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -569,7 +581,41 @@
         <v>0</v>
       </c>
       <c r="E6" t="s">
-        <v>14</v>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>